<commit_message>
atualizado planilha de gastor
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\Variado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
     <sheet name="Dezembro" sheetId="2" r:id="rId2"/>
     <sheet name="Janeiro" sheetId="3" r:id="rId3"/>
+    <sheet name="Fevereiro" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>kit placa mae + processador + memoria</t>
   </si>
@@ -191,14 +192,33 @@
   </si>
   <si>
     <t>bonecos naruto - Aliexpress</t>
+  </si>
+  <si>
+    <t>Compras 02/2021</t>
+  </si>
+  <si>
+    <t>Cartão SD</t>
+  </si>
+  <si>
+    <t>Capa flip iPhone 5s</t>
+  </si>
+  <si>
+    <t>Violino elétrico</t>
+  </si>
+  <si>
+    <t>Organizador de cabos</t>
+  </si>
+  <si>
+    <t>IPTU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -268,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -290,6 +310,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -576,7 +600,88 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5772150" y="466724"/>
+          <a:off x="5953125" y="466724"/>
+          <a:ext cx="876300" cy="840429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1219201</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>100965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7896226" y="390525"/>
+          <a:ext cx="914400" cy="853440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>107003</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4772025" y="409574"/>
           <a:ext cx="876300" cy="840429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1240,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1385,7 @@
       </c>
       <c r="F2" s="3">
         <f>SUM(B2:B29)</f>
-        <v>1707.15</v>
+        <v>1926.15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1371,7 +1476,7 @@
       </c>
       <c r="F11" s="3">
         <f>SUM(C2:C23)</f>
-        <v>765.01</v>
+        <v>546.01</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1394,7 +1499,7 @@
       <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="1">
+      <c r="B14" s="1">
         <v>124</v>
       </c>
     </row>
@@ -1402,7 +1507,7 @@
       <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="1">
+      <c r="B15" s="1">
         <v>95</v>
       </c>
     </row>
@@ -1420,6 +1525,141 @@
       </c>
       <c r="C17" s="1">
         <v>77.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1">
+        <v>65.69</v>
+      </c>
+      <c r="F2" s="10">
+        <f>SUM(B:B)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>44</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="10">
+        <v>109</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="10">
+        <v>32.89</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="10">
+        <v>64.34</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="10">
+        <v>640</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="10">
+        <v>631.52</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="10">
+        <f>SUM(C:C)</f>
+        <v>1619.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizado planilha de gastos
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>kit placa mae + processador + memoria</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>IPTU</t>
+  </si>
+  <si>
+    <t>Blusas mãe</t>
   </si>
 </sst>
 </file>
@@ -304,16 +307,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1037,13 +1040,13 @@
       <c r="B6" s="1">
         <v>120</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1052,11 +1055,11 @@
       <c r="B7" s="1">
         <v>56</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1065,11 +1068,11 @@
       <c r="B8" s="1">
         <v>150</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1078,11 +1081,11 @@
       <c r="B9" s="1">
         <v>44</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1251,10 +1254,10 @@
       <c r="B7" s="1">
         <v>20.98</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1263,8 +1266,8 @@
       <c r="B8" s="1">
         <v>496.84</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1273,8 +1276,8 @@
       <c r="B9" s="1">
         <v>33.89</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1286,8 +1289,8 @@
       <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1296,8 +1299,8 @@
       <c r="B11" s="1">
         <v>155.31</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1395,10 +1398,10 @@
       <c r="B3" s="1">
         <v>65</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1407,8 +1410,8 @@
       <c r="C4" s="1">
         <v>74.900000000000006</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1417,8 +1420,8 @@
       <c r="C5" s="1">
         <v>44</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1427,8 +1430,8 @@
       <c r="B6" s="1">
         <v>466.77</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1437,8 +1440,8 @@
       <c r="B7" s="1">
         <v>571.36</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1541,34 +1544,34 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1579,9 +1582,9 @@
       <c r="C2" s="1">
         <v>65.69</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <f>SUM(B:B)</f>
-        <v>0</v>
+        <v>665.16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1592,56 +1595,56 @@
       <c r="C3" s="1">
         <v>44</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>109</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="10">
+      <c r="B5" s="8">
         <v>32.89</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>64.34</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="10">
-        <v>640</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="B7" s="8">
+        <v>467.75</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>32</v>
       </c>
     </row>
@@ -1649,7 +1652,7 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>631.52</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1657,9 +1660,15 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="10">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="8">
+        <v>164.52</v>
+      </c>
+      <c r="F10" s="8">
         <f>SUM(C:C)</f>
-        <v>1619.44</v>
+        <v>946.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incluido lista rpgpc e atualizado planilha de gastos
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\Variado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\Variado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>kit placa mae + processador + memoria</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Blusas mãe</t>
+  </si>
+  <si>
+    <t>Balança digital</t>
+  </si>
+  <si>
+    <t>Motorola One</t>
   </si>
 </sst>
 </file>
@@ -1541,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1674,23 @@
       </c>
       <c r="F10" s="8">
         <f>SUM(C:C)</f>
-        <v>946.55</v>
+        <v>1872.55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="8">
+        <v>850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizado lista de gastos e incluido aquivos da pos ead
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\Variado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\Variado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>kit placa mae + processador + memoria</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>PosEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placa de Video </t>
+  </si>
+  <si>
+    <t>Adaptador Dvi / Vga</t>
   </si>
 </sst>
 </file>
@@ -1550,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1599,7 @@
       </c>
       <c r="F2" s="8">
         <f>SUM(B:B)</f>
-        <v>2187.41</v>
+        <v>2288.21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,6 +1708,22 @@
       </c>
       <c r="B13" s="8">
         <v>210.83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="8">
+        <v>20.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizado lista de gastos
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\Variado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\Variado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>kit placa mae + processador + memoria</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>PosEad - Big Data</t>
+  </si>
+  <si>
+    <t>Chip Fluke</t>
+  </si>
+  <si>
+    <t>Loterias CEF</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1653,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1693,7 @@
       </c>
       <c r="F2" s="8">
         <f>SUM(B:B)</f>
-        <v>2382.11</v>
+        <v>2382.02</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1718,7 +1724,7 @@
         <v>57</v>
       </c>
       <c r="B5" s="8">
-        <v>32.89</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1833,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,7 +1883,7 @@
       </c>
       <c r="F2" s="8">
         <f>SUM(B:B)</f>
-        <v>210.83</v>
+        <v>398.30000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1901,8 +1907,8 @@
       <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="8">
-        <v>109</v>
+      <c r="B5" s="8">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,9 +1923,23 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="8">
+        <v>26.97</v>
+      </c>
       <c r="F7" s="8">
         <f>SUM(C:C)</f>
-        <v>283.02999999999997</v>
+        <v>174.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="8">
+        <v>34.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incluido atualizacao da planilha de gastos e arquivos da pos ead
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\Variado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\Variado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="613" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,27 @@
     <sheet name="Fevereiro" sheetId="4" r:id="rId4"/>
     <sheet name="Março" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Não gasto</t>
+  </si>
+  <si>
+    <t>Total Gasto</t>
+  </si>
+  <si>
+    <t>À Gastar</t>
+  </si>
   <si>
     <t>kit placa mae + processador + memoria</t>
   </si>
@@ -45,6 +55,9 @@
     <t xml:space="preserve">teclado com led </t>
   </si>
   <si>
+    <t>Compras 11/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">mouse com led </t>
   </si>
   <si>
@@ -60,19 +73,7 @@
     <t xml:space="preserve">hub micro usb tablet </t>
   </si>
   <si>
-    <t>Produto</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Total Gasto</t>
-  </si>
-  <si>
-    <t>Não gasto</t>
-  </si>
-  <si>
-    <t>Compras 11/2020</t>
+    <t>tela iphone 5s</t>
   </si>
   <si>
     <t>vaso action figure</t>
@@ -81,12 +82,6 @@
     <t>perfume Luck</t>
   </si>
   <si>
-    <t>À Gastar</t>
-  </si>
-  <si>
-    <t>tela iphone 5s</t>
-  </si>
-  <si>
     <t>camiseta aliexpress</t>
   </si>
   <si>
@@ -96,6 +91,9 @@
     <t>Surface Pro I</t>
   </si>
   <si>
+    <t>Observação</t>
+  </si>
+  <si>
     <t>Jogo da Mesada</t>
   </si>
   <si>
@@ -114,6 +112,9 @@
     <t>Cartão SD Shopee</t>
   </si>
   <si>
+    <t>Compras 12/2020</t>
+  </si>
+  <si>
     <t>Placa mãe Xiaomi note 8 pro</t>
   </si>
   <si>
@@ -123,15 +124,9 @@
     <t>Samurai Jack Steam</t>
   </si>
   <si>
-    <t>Observação</t>
-  </si>
-  <si>
     <t>Promoção válido 05/01</t>
   </si>
   <si>
-    <t>Compras 12/2020</t>
-  </si>
-  <si>
     <t>Teclado bluetooh aliexpress</t>
   </si>
   <si>
@@ -156,15 +151,18 @@
     <t>Compras 01/2021</t>
   </si>
   <si>
+    <t>Teclado Notebook Compaq CQ40</t>
+  </si>
+  <si>
     <t>Desodorante kaik urbe</t>
   </si>
   <si>
+    <t>IPVA e Licenciamento Celta</t>
+  </si>
+  <si>
     <t>IPVA Prisma</t>
   </si>
   <si>
-    <t>IPVA e Licenciamento Celta</t>
-  </si>
-  <si>
     <t>Aliexpress Mãe</t>
   </si>
   <si>
@@ -180,18 +178,15 @@
     <t>Bateria Notebook Compaq CQ40</t>
   </si>
   <si>
-    <t>Teclado Notebook Compaq CQ40</t>
-  </si>
-  <si>
     <t>cinta modeladora</t>
   </si>
   <si>
+    <t>bateria sony xa1 - Aliexpress</t>
+  </si>
+  <si>
     <t>cartão sd 128 gb</t>
   </si>
   <si>
-    <t>bateria sony xa1 - Aliexpress</t>
-  </si>
-  <si>
     <t>bonecos naruto - Aliexpress</t>
   </si>
   <si>
@@ -241,6 +236,24 @@
   </si>
   <si>
     <t>Loterias CEF</t>
+  </si>
+  <si>
+    <t>Rifa templo</t>
+  </si>
+  <si>
+    <t>Memoria 2gb 1333Mhz</t>
+  </si>
+  <si>
+    <t>Pendrive 32Gb</t>
+  </si>
+  <si>
+    <t>Earth Defense - Steam</t>
+  </si>
+  <si>
+    <t>Wish</t>
+  </si>
+  <si>
+    <t>Compras 03/2021</t>
   </si>
 </sst>
 </file>
@@ -248,54 +261,52 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;&quot;-R$&quot;* #,##0.00_-;_-&quot;R$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -315,39 +326,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="3">
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,78 +379,166 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>257176</xdr:colOff>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>15241</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="1033" name="Imagem 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8067676" y="1066801"/>
-          <a:ext cx="914400" cy="853440"/>
+          <a:off x="8963025" y="876300"/>
+          <a:ext cx="857250" cy="847725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:colOff>971550</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>135579</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="1034" name="Imagem 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5219700" y="1200150"/>
-          <a:ext cx="876300" cy="840429"/>
+          <a:off x="5267325" y="1009650"/>
+          <a:ext cx="828675" cy="847725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -446,116 +548,248 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>120015</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="2061" name="Imagem 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8915401" y="1171575"/>
-          <a:ext cx="914400" cy="853440"/>
+          <a:off x="8963025" y="1162050"/>
+          <a:ext cx="857250" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>154628</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="2062" name="Imagem 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6038850" y="1219199"/>
-          <a:ext cx="876300" cy="840429"/>
+          <a:off x="6096000" y="1219200"/>
+          <a:ext cx="885825" cy="847725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1066999</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>181129</xdr:rowOff>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="2063" name="Imagem 3"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7134225" y="2124075"/>
-          <a:ext cx="1428949" cy="1105054"/>
+          <a:off x="7191375" y="2114550"/>
+          <a:ext cx="1352550" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -565,78 +799,166 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="3081" name="Imagem 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8772526" y="304800"/>
-          <a:ext cx="914400" cy="853440"/>
+          <a:off x="9001125" y="304800"/>
+          <a:ext cx="857250" cy="847725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
+      <xdr:colOff>895350</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>164153</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3082" name="Imagem 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5953125" y="466724"/>
-          <a:ext cx="876300" cy="840429"/>
+          <a:off x="6010275" y="466725"/>
+          <a:ext cx="838200" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -646,78 +968,166 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1219201</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>100965</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="4105" name="Imagem 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7896226" y="390525"/>
-          <a:ext cx="914400" cy="853440"/>
+          <a:off x="8458200" y="381000"/>
+          <a:ext cx="66675" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
+      <xdr:colOff>876300</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>107003</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="4106" name="Imagem 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4772025" y="409574"/>
-          <a:ext cx="876300" cy="840429"/>
+          <a:off x="4972050" y="400050"/>
+          <a:ext cx="828675" cy="847725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -727,78 +1137,166 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>95251</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>100965</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="5129" name="Imagem 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6953251" y="200025"/>
-          <a:ext cx="914400" cy="853440"/>
+          <a:off x="8048625" y="323850"/>
+          <a:ext cx="914400" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>97478</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="5130" name="Imagem 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4476750" y="209549"/>
-          <a:ext cx="876300" cy="840429"/>
+          <a:off x="5162550" y="438150"/>
+          <a:ext cx="828675" cy="752475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:blipFill dpi="0" rotWithShape="0">
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+                <a:srcRect/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1057,7 +1555,92 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1" cy="1"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:lstStyle/>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1" cy="1"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:lstStyle/>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -1075,198 +1658,202 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1"/>
+    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>400</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <f>SUM(B2:B22)</f>
         <v>2809.58</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <f>SUM(C2:C22)</f>
         <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
         <v>64.78</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
         <v>120</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>56</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>150</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>56</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>150</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
         <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1">
-        <v>52.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>1450</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="E6:I9"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.51180555555555551" right="0.51180555555555551" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1278,178 +1865,182 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
         <v>88.8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <f>SUM(B2:B21)</f>
         <v>1754.25</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <f>SUM(C2:C21)</f>
         <v>87.2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
         <v>144.9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2">
         <v>211.11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
         <v>43.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2">
         <v>20.98</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>496.84</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2">
+        <v>33.89</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2">
+        <v>52.84</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1">
-        <v>496.84</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1">
-        <v>33.89</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1">
-        <v>52.84</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>155.31</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>69.28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>235.9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>82.9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>87.2</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="F7:G11"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.51180555555555551" right="0.51180555555555551" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1461,189 +2052,193 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>12</v>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>65.69</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <f>SUM(B2:B29)</f>
         <v>1926.15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>65</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2">
         <v>74.900000000000006</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2">
         <v>44</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>466.77</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2">
         <v>571.36</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2">
         <v>222.72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>54.8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2">
         <v>167.8</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>17</v>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2">
         <v>120</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <f>SUM(C2:C23)</f>
         <v>546.01</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2">
         <v>38.700000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2">
         <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>77.42</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="F3:G7"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51180555555555551" right="0.51180555555555551" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1653,42 +2248,43 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F3" sqref="F3:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>12</v>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>65.69</v>
       </c>
       <c r="F2" s="8">
@@ -1697,60 +2293,60 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
         <v>44</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="8">
         <v>109</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="8">
         <v>32.799999999999997</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="8">
         <v>64.34</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="8">
         <v>467.75</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="8">
@@ -1758,18 +2354,18 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="8">
         <v>631.52</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
+      <c r="F9" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="8">
@@ -1781,7 +2377,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="8">
@@ -1789,7 +2385,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="8">
@@ -1797,7 +2393,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B13" s="8">
@@ -1805,7 +2401,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="8">
@@ -1813,7 +2409,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="8">
@@ -1821,7 +2417,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="8">
@@ -1829,53 +2425,57 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="F3:G7"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51180555555555551" right="0.51180555555555551" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="0.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="0.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="8">
@@ -1883,67 +2483,114 @@
       </c>
       <c r="F2" s="8">
         <f>SUM(B:B)</f>
-        <v>398.30000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>746.43000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>65.69</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1">
+      <c r="F3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="8">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="8">
-        <v>64.34</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B6" s="8">
+        <v>31</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B7" s="8">
-        <v>26.97</v>
-      </c>
-      <c r="F7" s="8">
+        <v>34.5</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="8">
+        <v>150</v>
+      </c>
+      <c r="F8" s="8">
         <f>SUM(C:C)</f>
-        <v>174.03</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="8">
-        <v>34.5</v>
+        <v>109.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="8">
+        <v>72.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="8">
+        <v>49.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="8">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="8">
+        <v>51.81</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.51180555555555551" right="0.51180555555555551" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
incluido arquivos da pos ead e atualizado planilha de gastos
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Fevereiro" sheetId="4" r:id="rId4"/>
     <sheet name="Março" sheetId="5" r:id="rId5"/>
     <sheet name="Abril" sheetId="6" r:id="rId6"/>
+    <sheet name="Maio" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
   <si>
     <t>Produto</t>
   </si>
@@ -335,6 +336,27 @@
   </si>
   <si>
     <t>Shopee</t>
+  </si>
+  <si>
+    <t>Compras 04/2021</t>
+  </si>
+  <si>
+    <t>Compras 05/2021</t>
+  </si>
+  <si>
+    <t>Steam Marvel</t>
+  </si>
+  <si>
+    <t>Pelicila motorola gshield</t>
+  </si>
+  <si>
+    <t>Pelicila motorola Mercado Livre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultra PC Compact </t>
+  </si>
+  <si>
+    <t>BB VT</t>
   </si>
 </sst>
 </file>
@@ -1003,6 +1025,122 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323115</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8115375" y="342900"/>
+          <a:ext cx="913590" cy="761280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1971135</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="390765"/>
+          <a:ext cx="828135" cy="751920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>56610</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6162675" y="438390"/>
+          <a:ext cx="828135" cy="751920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1656,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ17"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1837,7 @@
       </c>
       <c r="F2" s="6">
         <f>SUM(B2:B29)</f>
-        <v>1926.15</v>
+        <v>2136.98</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,6 +1977,14 @@
       </c>
       <c r="C17" s="2">
         <v>77.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="8">
+        <v>210.83</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +2002,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G7"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,7 +2193,7 @@
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2235,7 @@
       </c>
       <c r="F2" s="8">
         <f>SUM(B:B)</f>
-        <v>2546.4399999999996</v>
+        <v>2757.2699999999995</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2291,6 +2437,12 @@
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="8">
+        <v>210.83</v>
+      </c>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,10 +2490,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2381,7 +2533,7 @@
       </c>
       <c r="F2" s="13">
         <f>SUM(B:B)</f>
-        <v>2029.69</v>
+        <v>2240.52</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2395,7 +2547,7 @@
         <v>95</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="G3" s="19"/>
     </row>
@@ -2487,6 +2639,178 @@
         <v>258.99</v>
       </c>
       <c r="D11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="8">
+        <v>210.83</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" s="13">
+        <f>SUM(B:B)</f>
+        <v>2532.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1637.27</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8">
+        <v>210.83</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="13">
+        <v>278.89999999999998</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="13">
+        <v>33.880000000000003</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="13">
+        <v>29.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="13">
+        <v>60</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6.14</v>
+      </c>
+      <c r="F10" s="13">
+        <f>SUM(C:C)</f>
+        <v>462.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14">
+        <v>98.29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14">
+        <v>364.39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="14">
+        <v>275.33</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incluido arquivos da posead e atualizado planilha de gastos
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="125">
   <si>
     <t>Produto</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Desodorante Kaik</t>
+  </si>
+  <si>
+    <t>Cooler Led</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +1973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
@@ -2366,7 +2369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
@@ -2838,7 +2841,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3060,10 +3063,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3107,7 +3110,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="9">
         <f>SUM(B:B)</f>
-        <v>267.52</v>
+        <v>1071.02</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3136,8 +3139,8 @@
       <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="13">
-        <v>250</v>
+      <c r="B5" s="13">
+        <v>339.49</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -3146,8 +3149,8 @@
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="13">
-        <v>124</v>
+      <c r="B6" s="13">
+        <v>123</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -3156,8 +3159,8 @@
       <c r="A7" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="13">
-        <v>82</v>
+      <c r="B7" s="13">
+        <v>81.72</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -3182,9 +3185,23 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="13">
+        <v>48.46</v>
+      </c>
       <c r="F10" s="13">
         <f>SUM(C:C)</f>
-        <v>546</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="13">
+        <v>210.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incluido drive da impressora e atualizado planilha de gastos
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\Variado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\Variado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Abril" sheetId="6" r:id="rId6"/>
     <sheet name="Maio" sheetId="7" r:id="rId7"/>
     <sheet name="Junho" sheetId="8" r:id="rId8"/>
+    <sheet name="Julho" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="133">
   <si>
     <t>Produto</t>
   </si>
@@ -418,6 +419,18 @@
   </si>
   <si>
     <t>Mini ventilador</t>
+  </si>
+  <si>
+    <t>Steam - 4 jogos</t>
+  </si>
+  <si>
+    <t>Compras 07/2021</t>
+  </si>
+  <si>
+    <t>Compras 06/2021</t>
+  </si>
+  <si>
+    <t>Playstore</t>
   </si>
 </sst>
 </file>
@@ -1294,6 +1307,85 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285824</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>151680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334449" y="333375"/>
+          <a:ext cx="952425" cy="980355"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28035</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5372100" y="447675"/>
+          <a:ext cx="894810" cy="742636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -3041,8 +3133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3097,7 +3189,7 @@
         <v>51.84</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="G3" s="22"/>
     </row>
@@ -3220,4 +3312,106 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="13">
+        <v>124.9</v>
+      </c>
+      <c r="F2" s="13">
+        <f>SUM(B:B)</f>
+        <v>218.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="13">
+        <v>75.56</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="13">
+        <v>17.79</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" s="13">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
atualizado lista de gastos e incluido exemplo imagem alerta bb
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Maio" sheetId="7" r:id="rId7"/>
     <sheet name="Junho" sheetId="8" r:id="rId8"/>
     <sheet name="Julho" sheetId="9" r:id="rId9"/>
+    <sheet name="Agosto" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="147">
   <si>
     <t>Produto</t>
   </si>
@@ -443,6 +444,36 @@
   </si>
   <si>
     <t>Bateria iPhone 6s</t>
+  </si>
+  <si>
+    <t>Colar akatsuki</t>
+  </si>
+  <si>
+    <t>Pulseira akatsuki</t>
+  </si>
+  <si>
+    <t>Compras 08/2021</t>
+  </si>
+  <si>
+    <t>Fone bluetooth</t>
+  </si>
+  <si>
+    <t>Headset bluetooth</t>
+  </si>
+  <si>
+    <t>Controle USB Xbox -&gt; PC</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Chassi iPhone 6s</t>
+  </si>
+  <si>
+    <t>Caixa loterias</t>
+  </si>
+  <si>
+    <t>Sony Xperia L4</t>
   </si>
 </sst>
 </file>
@@ -678,6 +709,85 @@
         <a:xfrm>
           <a:off x="5564880" y="1009440"/>
           <a:ext cx="828000" cy="847080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28035</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5514975" y="447675"/>
+          <a:ext cx="894810" cy="742636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>75480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8162925" y="257175"/>
+          <a:ext cx="952425" cy="980355"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1864,6 +1974,161 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="15" style="13" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="13">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="13">
+        <f>SUM(B:B)</f>
+        <v>1461.86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="13">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="13">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="13">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="13">
+        <v>210.83</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="13">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="13">
+        <v>157.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="13">
+        <v>39</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1054.5999999999999</v>
+      </c>
+      <c r="F10" s="13">
+        <f>SUM(C:C)</f>
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ15"/>
@@ -3330,8 +3595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
incluido arquivos da pos ead de big data
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Junho" sheetId="8" r:id="rId8"/>
     <sheet name="Julho" sheetId="9" r:id="rId9"/>
     <sheet name="Agosto" sheetId="10" r:id="rId10"/>
+    <sheet name="Setembro" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="159">
   <si>
     <t>Produto</t>
   </si>
@@ -498,6 +499,18 @@
   </si>
   <si>
     <t>Taxa Sony L4</t>
+  </si>
+  <si>
+    <t>Compras 09/2021</t>
+  </si>
+  <si>
+    <t>Roupas (camisas e calça)</t>
+  </si>
+  <si>
+    <t>Caedu</t>
+  </si>
+  <si>
+    <t>Fonte Surface Pro</t>
   </si>
 </sst>
 </file>
@@ -812,6 +825,85 @@
         <a:xfrm>
           <a:off x="8162925" y="257175"/>
           <a:ext cx="952425" cy="980355"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28035</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="447675"/>
+          <a:ext cx="1294860" cy="771211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7419975" y="371475"/>
+          <a:ext cx="952425" cy="885825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2002,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2202,6 +2294,111 @@
       </c>
       <c r="D16" t="s">
         <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13" style="13" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="13">
+        <v>225.71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="13">
+        <f>SUM(B:B)</f>
+        <v>601.54000000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="13">
+        <v>165</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="13">
+        <v>210.83</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" s="13">
+        <f>SUM(C:C)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incluido material da pos ead de big data
</commit_message>
<xml_diff>
--- a/Variado/Gastos2020-2021.xlsx
+++ b/Variado/Gastos2020-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Julho" sheetId="9" r:id="rId9"/>
     <sheet name="Agosto" sheetId="10" r:id="rId10"/>
     <sheet name="Setembro" sheetId="11" r:id="rId11"/>
+    <sheet name="Outubro" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="176">
   <si>
     <t>Produto</t>
   </si>
@@ -511,6 +512,57 @@
   </si>
   <si>
     <t>Fonte Surface Pro</t>
+  </si>
+  <si>
+    <t>Compras 10/2021</t>
+  </si>
+  <si>
+    <t>Roupas mãe</t>
+  </si>
+  <si>
+    <t>Capas Q20</t>
+  </si>
+  <si>
+    <t>Filtro e torneira</t>
+  </si>
+  <si>
+    <t>Película Q20</t>
+  </si>
+  <si>
+    <t>Teclado &amp; Mouse</t>
+  </si>
+  <si>
+    <t>Mini PC</t>
+  </si>
+  <si>
+    <t>Ulefone Note 6P</t>
+  </si>
+  <si>
+    <t>Pelucia Livia</t>
+  </si>
+  <si>
+    <t>Irrigador Portátil</t>
+  </si>
+  <si>
+    <t>Fone Bluetooth</t>
+  </si>
+  <si>
+    <t>Capa Positivo Q20</t>
+  </si>
+  <si>
+    <t>Squeeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protetor Orelha </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Palmilha Tenis</t>
+  </si>
+  <si>
+    <t>Webcam</t>
   </si>
 </sst>
 </file>
@@ -523,7 +575,7 @@
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * \-??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -587,6 +639,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -610,7 +668,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -661,6 +719,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -844,15 +908,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>28035</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28261</xdr:rowOff>
+      <xdr:colOff>132810</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -865,8 +929,87 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4953000" y="447675"/>
-          <a:ext cx="1294860" cy="771211"/>
+          <a:off x="4600575" y="409575"/>
+          <a:ext cx="1113885" cy="771211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8010525" y="352425"/>
+          <a:ext cx="952425" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1342485</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152086</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4476750" y="381000"/>
+          <a:ext cx="1113885" cy="771211"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -881,15 +1024,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>228525</xdr:colOff>
+      <xdr:colOff>333300</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -902,8 +1045,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7419975" y="371475"/>
-          <a:ext cx="952425" cy="885825"/>
+          <a:off x="7600950" y="333375"/>
+          <a:ext cx="952425" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2094,7 +2237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2353,7 +2496,7 @@
       </c>
       <c r="F2" s="13">
         <f>SUM(B:B)</f>
-        <v>601.54000000000008</v>
+        <v>1157.9100000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2379,16 +2522,51 @@
       <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="13">
+        <v>334.44</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="13">
+        <v>48.12</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="13">
+        <v>83.91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="13">
+        <v>89.9</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F9" s="17" t="s">
@@ -2407,6 +2585,200 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="23">
+        <v>210.83</v>
+      </c>
+      <c r="F2" s="13">
+        <f>SUM(B:B)</f>
+        <v>492.55999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="13">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="13">
+        <v>900</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="13">
+        <v>498</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="23">
+        <v>130.07</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="13">
+        <v>82.62</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="24">
+        <v>123.66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="13">
+        <v>149</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="13">
+        <v>89</v>
+      </c>
+      <c r="F10" s="13">
+        <f>SUM(C:C)</f>
+        <v>2000.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="13">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="13">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="13">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>